<commit_message>
fix sheet name error
</commit_message>
<xml_diff>
--- a/jpaexl.xlsx
+++ b/jpaexl.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="String" r:id="rId3" sheetId="1"/>
+    <sheet name="Dummy" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -177,4 +178,22 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add maven publishing setting
</commit_message>
<xml_diff>
--- a/jpaexl.xlsx
+++ b/jpaexl.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -98,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -174,6 +174,174 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
save witout duplicated id
</commit_message>
<xml_diff>
--- a/jpaexl.xlsx
+++ b/jpaexl.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -110,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -201,6 +201,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>